<commit_message>
travail sur les lib (corrections+ homogeinisation des grilles) mise à jour de la liste des composants à créer (partielle)
</commit_message>
<xml_diff>
--- a/1-LIB/Composant_a_creer.xlsx
+++ b/1-LIB/Composant_a_creer.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Robotique 2018\ELEC\1-LIB\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="576" yWindow="96" windowWidth="29604" windowHeight="13776"/>
   </bookViews>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="188">
   <si>
     <t xml:space="preserve">code couleur: </t>
   </si>
@@ -416,9 +411,6 @@
     <t>pwr, cdc, prp</t>
   </si>
   <si>
-    <t>je dois vérifier l'empreinte</t>
-  </si>
-  <si>
     <t>ISO1050DUBR</t>
   </si>
   <si>
@@ -482,9 +474,6 @@
   </si>
   <si>
     <t>pour aller avec le composant ci-dessus, voir sa datasheet</t>
-  </si>
-  <si>
-    <t>La bobine n'est pas encore faite</t>
   </si>
   <si>
     <t>Wurth</t>
@@ -577,9 +566,6 @@
     <t>NX3008PBKS</t>
   </si>
   <si>
-    <t>INA139</t>
-  </si>
-  <si>
     <t>OPA340</t>
   </si>
   <si>
@@ -592,21 +578,65 @@
     <t>GoG_PWR</t>
   </si>
   <si>
-    <t>symbole incorrect, il manque la Part B (voir youtube: /watch?v=i6x7t1woQXc)</t>
+    <t>INA139NA/250</t>
   </si>
   <si>
-    <t>symbole incomplet: il manque la pin 9, le "Pad"</t>
+    <t>BAT54XV2</t>
   </si>
   <si>
-    <t>Il en existe deux versions possibles :  
-INA139NA/250 et INA139NA/3K ; je dois prendre laquelle ? (J'ai pris la 250).</t>
+    <t>fichier Step "SOD-523F" pour la 3D ajouté au répertoire "98_generic_component_3Dstep"</t>
+  </si>
+  <si>
+    <t>Diode</t>
+  </si>
+  <si>
+    <t>CaP_CDC</t>
+  </si>
+  <si>
+    <t>j'ai corrigé, mais 
+-le symbole était incorrect, il manquait la Part B (voir youtube: /watch?v=i6x7t1woQXc)
+- le Mosfet représenté n'est pas un P mais un N</t>
+  </si>
+  <si>
+    <t>-j'ai changé le 3D de l'empreinte
+- ce n'est pas CI? Mais U?</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>a rangé dans la lib CI et non AOP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (penser à mettre à jour les composants dans les schémas)
+- j'ai changé le 3D de l'empreinte
+- ce n'est pas CI? Mais U?</t>
+    </r>
+  </si>
+  <si>
+    <t>- pin de 20 et non de 30.
+- pin en "passive"</t>
+  </si>
+  <si>
+    <t>La bobine n'est pas encore faite, wurth 74404020022? (c'est ce qui est sur la carte en ce moment)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -653,6 +683,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFCC0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -823,7 +860,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -948,6 +985,9 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1008,7 +1048,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1041,26 +1081,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1093,23 +1116,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1288,8 +1294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2975,10 +2981,10 @@
         <v>31</v>
       </c>
       <c r="L35" s="33">
-        <v>42799</v>
-      </c>
-      <c r="M35" s="3" t="s">
-        <v>124</v>
+        <v>43170</v>
+      </c>
+      <c r="M35" s="46" t="s">
+        <v>186</v>
       </c>
       <c r="N35" s="3" t="s">
         <v>33</v>
@@ -3000,22 +3006,22 @@
     </row>
     <row r="36" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="C36" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="D36" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>26</v>
@@ -3046,22 +3052,22 @@
     </row>
     <row r="37" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C37" s="1" t="s">
+      <c r="D37" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>132</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>26</v>
@@ -3095,13 +3101,13 @@
         <v>605240</v>
       </c>
       <c r="C38" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="E38" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>111</v>
@@ -3141,7 +3147,7 @@
     </row>
     <row r="39" spans="1:28" ht="72" x14ac:dyDescent="0.3">
       <c r="A39" s="30" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>100</v>
@@ -3161,7 +3167,7 @@
       <c r="K39" s="2"/>
       <c r="L39" s="33"/>
       <c r="M39" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N39" s="3"/>
       <c r="O39" s="3"/>
@@ -3181,17 +3187,17 @@
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A40" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>142</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>117</v>
@@ -3227,13 +3233,13 @@
       <c r="AA40" s="3"/>
       <c r="AB40" s="3"/>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -3245,7 +3251,7 @@
       <c r="K41" s="2"/>
       <c r="L41" s="33"/>
       <c r="M41" s="3" t="s">
-        <v>145</v>
+        <v>187</v>
       </c>
       <c r="N41" s="3"/>
       <c r="O41" s="3"/>
@@ -3268,17 +3274,17 @@
         <v>61300311021</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E42" s="21" t="s">
         <v>103</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>26</v>
@@ -3318,38 +3324,42 @@
       <c r="AB42" s="3"/>
     </row>
     <row r="43" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A43" s="9" t="s">
-        <v>149</v>
+      <c r="A43" s="27" t="s">
+        <v>147</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="1"/>
       <c r="D43" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H43" s="33"/>
+      <c r="H43" s="33">
+        <v>42805</v>
+      </c>
       <c r="I43" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J43" s="33"/>
+        <v>27</v>
+      </c>
+      <c r="J43" s="33">
+        <v>43170</v>
+      </c>
       <c r="K43" s="2" t="s">
         <v>31</v>
       </c>
       <c r="L43" s="33">
         <v>43108</v>
       </c>
-      <c r="M43" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="N43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="O43" s="3"/>
       <c r="P43" s="3"/>
       <c r="Q43" s="3"/>
@@ -3370,10 +3380,10 @@
         <v>158301227</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>29</v>
@@ -3382,7 +3392,7 @@
         <v>30</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>26</v>
@@ -3420,11 +3430,11 @@
         <v>418121270808</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>119</v>
@@ -3472,17 +3482,17 @@
         <v>82401646</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>26</v>
@@ -3526,19 +3536,19 @@
         <v>452403012014</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>119</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>26</v>
@@ -3582,11 +3592,11 @@
         <v>824540241</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>95</v>
@@ -3633,7 +3643,7 @@
     </row>
     <row r="49" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A49" s="27" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="1"/>
@@ -3685,12 +3695,12 @@
     </row>
     <row r="50" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A50" s="27" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="1"/>
       <c r="D50" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>85</v>
@@ -3717,7 +3727,7 @@
         <v>42806</v>
       </c>
       <c r="M50" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="N50" s="3" t="s">
         <v>33</v>
@@ -3742,11 +3752,11 @@
         <v>691322110006</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>103</v>
@@ -3796,11 +3806,11 @@
         <v>691322110002</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>103</v>
@@ -3850,17 +3860,17 @@
         <v>691322110003</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>103</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>26</v>
@@ -3901,14 +3911,14 @@
     </row>
     <row r="54" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A54" s="27" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>103</v>
@@ -3955,17 +3965,17 @@
     </row>
     <row r="55" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A55" s="28" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>53</v>
@@ -4001,9 +4011,9 @@
       <c r="AA55" s="3"/>
       <c r="AB55" s="3"/>
     </row>
-    <row r="56" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A56" s="9" t="s">
-        <v>175</v>
+    <row r="56" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A56" s="27" t="s">
+        <v>173</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="1"/>
@@ -4035,9 +4045,11 @@
         <v>43108</v>
       </c>
       <c r="M56" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="N56" s="3"/>
+        <v>183</v>
+      </c>
+      <c r="N56" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="O56" s="3"/>
       <c r="P56" s="3"/>
       <c r="Q56" s="3"/>
@@ -4053,22 +4065,20 @@
       <c r="AA56" s="3"/>
       <c r="AB56" s="3"/>
     </row>
-    <row r="57" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A57" s="31" t="s">
-        <v>176</v>
+    <row r="57" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A57" s="27" t="s">
+        <v>178</v>
       </c>
       <c r="B57" s="2"/>
-      <c r="C57" s="1" t="s">
-        <v>183</v>
-      </c>
+      <c r="C57" s="1"/>
       <c r="D57" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>56</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>26</v>
@@ -4082,10 +4092,18 @@
       <c r="J57" s="33">
         <v>43122</v>
       </c>
-      <c r="K57" s="2"/>
-      <c r="L57" s="33"/>
-      <c r="M57" s="3"/>
-      <c r="N57" s="3"/>
+      <c r="K57" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L57" s="33">
+        <v>43170</v>
+      </c>
+      <c r="M57" s="46" t="s">
+        <v>184</v>
+      </c>
+      <c r="N57" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="O57" s="3"/>
       <c r="P57" s="3"/>
       <c r="Q57" s="3"/>
@@ -4101,22 +4119,20 @@
       <c r="AA57" s="3"/>
       <c r="AB57" s="3"/>
     </row>
-    <row r="58" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A58" s="31" t="s">
+    <row r="58" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A58" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="B58" s="2"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="F58" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="B58" s="2"/>
-      <c r="C58" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>180</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>26</v>
@@ -4130,9 +4146,15 @@
       <c r="J58" s="33">
         <v>43122</v>
       </c>
-      <c r="K58" s="2"/>
-      <c r="L58" s="33"/>
-      <c r="M58" s="3"/>
+      <c r="K58" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L58" s="33">
+        <v>43170</v>
+      </c>
+      <c r="M58" s="3" t="s">
+        <v>185</v>
+      </c>
       <c r="N58" s="3"/>
       <c r="O58" s="3"/>
       <c r="P58" s="3"/>
@@ -4149,13 +4171,23 @@
       <c r="AA58" s="3"/>
       <c r="AB58" s="3"/>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A59" s="32"/>
+    <row r="59" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A59" s="31" t="s">
+        <v>179</v>
+      </c>
       <c r="B59" s="2"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
+      <c r="C59" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>182</v>
+      </c>
       <c r="G59" s="2"/>
       <c r="H59" s="33"/>
       <c r="I59" s="2"/>

</xml_diff>

<commit_message>
mise en conformité de la lib diode
</commit_message>
<xml_diff>
--- a/1-LIB/Composant_a_creer.xlsx
+++ b/1-LIB/Composant_a_creer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\DOC\Audran\GIT\ELEC\1-LIB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF63740-538E-453B-90A2-1F2208E831B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF68D4C-853F-47A4-AA99-C3219AF6511E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-1365" windowWidth="38640" windowHeight="21840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="composant_a_creer" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="250">
   <si>
     <t xml:space="preserve">code couleur: </t>
   </si>
@@ -809,12 +809,6 @@
     <t>rangé dans la lib relays.schlib au lieu de Switches.schlib</t>
   </si>
   <si>
-    <t>le fichier schlib correspondant n'a pas été remonté</t>
-  </si>
-  <si>
-    <t>NOK</t>
-  </si>
-  <si>
     <t>HT7550-1</t>
   </si>
   <si>
@@ -831,6 +825,15 @@
   </si>
   <si>
     <t>Pince 2020</t>
+  </si>
+  <si>
+    <t>FT232RL-reel</t>
+  </si>
+  <si>
+    <t>Future Designs</t>
+  </si>
+  <si>
+    <t>USB-to-UART, associer JLCPCB C8690</t>
   </si>
 </sst>
 </file>
@@ -1029,7 +1032,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1176,6 +1179,12 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1188,10 +1197,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1580,8 +1589,8 @@
   <dimension ref="A1:AMJ1007"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D75" sqref="D75"/>
+      <pane ySplit="5" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1708,28 +1717,28 @@
       <c r="AB3" s="23"/>
     </row>
     <row r="4" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="51" t="s">
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="51"/>
-      <c r="I4" s="52" t="s">
+      <c r="H4" s="53"/>
+      <c r="I4" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="52"/>
-      <c r="K4" s="53" t="s">
+      <c r="J4" s="54"/>
+      <c r="K4" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="53"/>
-      <c r="M4" s="53"/>
-      <c r="N4" s="53"/>
+      <c r="L4" s="55"/>
+      <c r="M4" s="55"/>
+      <c r="N4" s="55"/>
       <c r="O4" s="22" t="s">
         <v>11</v>
       </c>
@@ -4942,25 +4951,25 @@
       <c r="AB69" s="10"/>
     </row>
     <row r="70" spans="1:28" ht="45" x14ac:dyDescent="0.25">
-      <c r="A70" s="15">
+      <c r="A70" s="12">
         <v>82400274</v>
       </c>
-      <c r="B70" s="54" t="s">
+      <c r="B70" s="56" t="s">
         <v>146</v>
       </c>
-      <c r="C70" s="55" t="s">
+      <c r="C70" s="57" t="s">
         <v>208</v>
       </c>
-      <c r="D70" s="54" t="s">
+      <c r="D70" s="56" t="s">
         <v>209</v>
       </c>
-      <c r="E70" s="54" t="s">
+      <c r="E70" s="56" t="s">
         <v>186</v>
       </c>
-      <c r="F70" s="54" t="s">
+      <c r="F70" s="56" t="s">
         <v>190</v>
       </c>
-      <c r="G70" s="54" t="s">
+      <c r="G70" s="56" t="s">
         <v>239</v>
       </c>
       <c r="H70" s="8"/>
@@ -4970,13 +4979,11 @@
         <v>27</v>
       </c>
       <c r="L70" s="8">
-        <v>43953</v>
-      </c>
-      <c r="M70" s="9" t="s">
-        <v>241</v>
-      </c>
+        <v>43954</v>
+      </c>
+      <c r="M70" s="9"/>
       <c r="N70" s="9" t="s">
-        <v>242</v>
+        <v>33</v>
       </c>
       <c r="O70" s="9"/>
       <c r="P70" s="10"/>
@@ -5627,13 +5634,13 @@
     </row>
     <row r="85" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="42" t="s">
+        <v>241</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="C85" s="6" t="s">
         <v>243</v>
-      </c>
-      <c r="B85" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>245</v>
       </c>
       <c r="D85" s="7" t="s">
         <v>232</v>
@@ -5642,7 +5649,7 @@
         <v>233</v>
       </c>
       <c r="F85" s="7" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G85" s="7"/>
       <c r="H85" s="8"/>
@@ -5669,21 +5676,21 @@
     </row>
     <row r="86" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="42" t="s">
-        <v>246</v>
-      </c>
-      <c r="B86" s="54" t="s">
         <v>244</v>
       </c>
-      <c r="C86" s="55" t="s">
-        <v>247</v>
-      </c>
-      <c r="D86" s="54" t="s">
+      <c r="B86" s="50" t="s">
+        <v>242</v>
+      </c>
+      <c r="C86" s="51" t="s">
+        <v>245</v>
+      </c>
+      <c r="D86" s="50" t="s">
         <v>232</v>
       </c>
-      <c r="E86" s="54" t="s">
+      <c r="E86" s="50" t="s">
         <v>233</v>
       </c>
-      <c r="F86" s="54" t="s">
+      <c r="F86" s="50" t="s">
         <v>190</v>
       </c>
       <c r="G86" s="7"/>
@@ -5709,13 +5716,25 @@
       <c r="AA86" s="10"/>
       <c r="AB86" s="10"/>
     </row>
-    <row r="87" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A87" s="49"/>
-      <c r="B87" s="7"/>
-      <c r="C87" s="6"/>
-      <c r="D87" s="7"/>
-      <c r="E87" s="7"/>
-      <c r="F87" s="7"/>
+    <row r="87" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" s="49" t="s">
+        <v>247</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="D87" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E87" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F87" s="7" t="s">
+        <v>229</v>
+      </c>
       <c r="G87" s="7"/>
       <c r="H87" s="8"/>
       <c r="I87" s="7"/>
@@ -33350,6 +33369,6 @@
     <hyperlink ref="C76" r:id="rId1" location="440GS67082622" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Part 2 de la  maj de la carte alimentation
</commit_message>
<xml_diff>
--- a/1-LIB/Composant_a_creer.xlsx
+++ b/1-LIB/Composant_a_creer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\DOC\Audran\GIT\ELEC\1-LIB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF68D4C-853F-47A4-AA99-C3219AF6511E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B0B0DA-B4ED-49D9-B90A-FE32609B2727}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-1365" windowWidth="38640" windowHeight="21840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="composant_a_creer" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="256">
   <si>
     <t xml:space="preserve">code couleur: </t>
   </si>
@@ -835,6 +835,24 @@
   <si>
     <t>USB-to-UART, associer JLCPCB C8690</t>
   </si>
+  <si>
+    <t>A3213EUA-T</t>
+  </si>
+  <si>
+    <t>Alegro</t>
+  </si>
+  <si>
+    <t>Capteur à effet Hall</t>
+  </si>
+  <si>
+    <t>HAL</t>
+  </si>
+  <si>
+    <t>l'association JLCPCB avait été oublié (ou perdue)</t>
+  </si>
+  <si>
+    <t>capa 10uF 25V JLCPCB C15850??</t>
+  </si>
 </sst>
 </file>
 
@@ -1032,7 +1050,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1185,6 +1203,15 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1196,12 +1223,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1589,8 +1610,8 @@
   <dimension ref="A1:AMJ1007"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C87" sqref="C87"/>
+      <pane ySplit="5" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1717,28 +1738,28 @@
       <c r="AB3" s="23"/>
     </row>
     <row r="4" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="53" t="s">
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="53"/>
-      <c r="I4" s="54" t="s">
+      <c r="H4" s="56"/>
+      <c r="I4" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="54"/>
-      <c r="K4" s="55" t="s">
+      <c r="J4" s="57"/>
+      <c r="K4" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="55"/>
-      <c r="M4" s="55"/>
-      <c r="N4" s="55"/>
+      <c r="L4" s="58"/>
+      <c r="M4" s="58"/>
+      <c r="N4" s="58"/>
       <c r="O4" s="22" t="s">
         <v>11</v>
       </c>
@@ -4954,22 +4975,22 @@
       <c r="A70" s="12">
         <v>82400274</v>
       </c>
-      <c r="B70" s="56" t="s">
+      <c r="B70" s="52" t="s">
         <v>146</v>
       </c>
-      <c r="C70" s="57" t="s">
+      <c r="C70" s="53" t="s">
         <v>208</v>
       </c>
-      <c r="D70" s="56" t="s">
+      <c r="D70" s="52" t="s">
         <v>209</v>
       </c>
-      <c r="E70" s="56" t="s">
+      <c r="E70" s="52" t="s">
         <v>186</v>
       </c>
-      <c r="F70" s="56" t="s">
+      <c r="F70" s="52" t="s">
         <v>190</v>
       </c>
-      <c r="G70" s="56" t="s">
+      <c r="G70" s="52" t="s">
         <v>239</v>
       </c>
       <c r="H70" s="8"/>
@@ -4981,7 +5002,9 @@
       <c r="L70" s="8">
         <v>43954</v>
       </c>
-      <c r="M70" s="9"/>
+      <c r="M70" s="9" t="s">
+        <v>254</v>
+      </c>
       <c r="N70" s="9" t="s">
         <v>33</v>
       </c>
@@ -5759,13 +5782,25 @@
       <c r="AB87" s="10"/>
     </row>
     <row r="88" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A88" s="49"/>
-      <c r="B88" s="7"/>
-      <c r="C88" s="6"/>
-      <c r="D88" s="7"/>
-      <c r="E88" s="7"/>
-      <c r="F88" s="7"/>
-      <c r="G88" s="7"/>
+      <c r="A88" s="49" t="s">
+        <v>250</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="D88" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="E88" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="F88" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="G88" s="54"/>
       <c r="H88" s="8"/>
       <c r="I88" s="7"/>
       <c r="J88" s="8"/>
@@ -5791,7 +5826,9 @@
     <row r="89" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A89" s="49"/>
       <c r="B89" s="7"/>
-      <c r="C89" s="6"/>
+      <c r="C89" s="6" t="s">
+        <v>255</v>
+      </c>
       <c r="D89" s="7"/>
       <c r="E89" s="7"/>
       <c r="F89" s="7"/>

</xml_diff>

<commit_message>
Maj lib condensateur (ménage, footprint, JLCPCB parts)
</commit_message>
<xml_diff>
--- a/1-LIB/Composant_a_creer.xlsx
+++ b/1-LIB/Composant_a_creer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\DOC\Audran\GIT\ELEC\1-LIB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACA0547-C29A-4089-8A53-80CE8BBE6E79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADCFB946-E06D-4D2E-B536-43EC364E667A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-1365" windowWidth="38640" windowHeight="21840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1203,9 +1203,6 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="12" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1217,6 +1214,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="12" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1604,8 +1604,8 @@
   <dimension ref="A1:AMJ1009"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M91" sqref="M91"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G88" sqref="G88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1732,28 +1732,28 @@
       <c r="AB3" s="23"/>
     </row>
     <row r="4" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="53" t="s">
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="53"/>
-      <c r="I4" s="54" t="s">
+      <c r="H4" s="52"/>
+      <c r="I4" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="54"/>
-      <c r="K4" s="55" t="s">
+      <c r="J4" s="53"/>
+      <c r="K4" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="55"/>
-      <c r="M4" s="55"/>
-      <c r="N4" s="55"/>
+      <c r="L4" s="54"/>
+      <c r="M4" s="54"/>
+      <c r="N4" s="54"/>
       <c r="O4" s="22" t="s">
         <v>11</v>
       </c>
@@ -5974,7 +5974,7 @@
       <c r="AB90" s="10"/>
     </row>
     <row r="91" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A91" s="51">
+      <c r="A91" s="55">
         <v>885012107010</v>
       </c>
       <c r="B91" s="7" t="s">

</xml_diff>

<commit_message>
Creation de la lib archive (trop de composant obsolete dans les lib, un peu de ménage)
</commit_message>
<xml_diff>
--- a/1-LIB/Composant_a_creer.xlsx
+++ b/1-LIB/Composant_a_creer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\DOC\Audran\GIT\ELEC\1-LIB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADCFB946-E06D-4D2E-B536-43EC364E667A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA039D6A-7A31-4724-950B-65A25E855F7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-1365" windowWidth="38640" windowHeight="21840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4455" yWindow="-120" windowWidth="28980" windowHeight="15930" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="composant_a_creer" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="265">
   <si>
     <t xml:space="preserve">code couleur: </t>
   </si>
@@ -868,6 +868,15 @@
   <si>
     <t xml:space="preserve">61000421821	</t>
   </si>
+  <si>
+    <t>SN74LVC1G17DBVR</t>
+  </si>
+  <si>
+    <t>Buffer non inverseur</t>
+  </si>
+  <si>
+    <t>OPB 2020</t>
+  </si>
 </sst>
 </file>
 
@@ -1203,6 +1212,9 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="12" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1214,9 +1226,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="12" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1604,8 +1613,8 @@
   <dimension ref="A1:AMJ1009"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G88" sqref="G88"/>
+      <pane ySplit="5" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1732,28 +1741,28 @@
       <c r="AB3" s="23"/>
     </row>
     <row r="4" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="52" t="s">
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="52"/>
-      <c r="I4" s="53" t="s">
+      <c r="H4" s="53"/>
+      <c r="I4" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="53"/>
-      <c r="K4" s="54" t="s">
+      <c r="J4" s="54"/>
+      <c r="K4" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="54"/>
-      <c r="M4" s="54"/>
-      <c r="N4" s="54"/>
+      <c r="L4" s="55"/>
+      <c r="M4" s="55"/>
+      <c r="N4" s="55"/>
       <c r="O4" s="22" t="s">
         <v>11</v>
       </c>
@@ -5974,7 +5983,7 @@
       <c r="AB90" s="10"/>
     </row>
     <row r="91" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A91" s="55">
+      <c r="A91" s="51">
         <v>885012107010</v>
       </c>
       <c r="B91" s="7" t="s">
@@ -6034,7 +6043,9 @@
       <c r="F92" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="G92" s="7"/>
+      <c r="G92" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="H92" s="8"/>
       <c r="I92" s="7"/>
       <c r="J92" s="8"/>
@@ -6058,14 +6069,30 @@
       <c r="AB92" s="10"/>
     </row>
     <row r="93" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A93" s="47"/>
-      <c r="B93" s="7"/>
-      <c r="C93" s="6"/>
-      <c r="D93" s="7"/>
-      <c r="E93" s="7"/>
-      <c r="F93" s="7"/>
-      <c r="G93" s="7"/>
-      <c r="H93" s="8"/>
+      <c r="A93" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="D93" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E93" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F93" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="G93" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H93" s="8">
+        <v>43978</v>
+      </c>
       <c r="I93" s="7"/>
       <c r="J93" s="8"/>
       <c r="K93" s="7"/>

</xml_diff>

<commit_message>
Suite de la mise en archive et mise à jour des libs
</commit_message>
<xml_diff>
--- a/1-LIB/Composant_a_creer.xlsx
+++ b/1-LIB/Composant_a_creer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\DOC\Audran\GIT\ELEC\1-LIB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA039D6A-7A31-4724-950B-65A25E855F7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5FA10F-50E4-4048-8C79-72E54CB34424}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4455" yWindow="-120" windowWidth="28980" windowHeight="15930" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="composant_a_creer" sheetId="1" r:id="rId1"/>
@@ -1613,8 +1613,8 @@
   <dimension ref="A1:AMJ1009"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B100" sqref="B100"/>
+      <pane ySplit="5" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fin de la mise à jour des bibliothèque de composant (sauf coquille).
</commit_message>
<xml_diff>
--- a/1-LIB/Composant_a_creer.xlsx
+++ b/1-LIB/Composant_a_creer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\DOC\Audran\GIT\ELEC\1-LIB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5FA10F-50E4-4048-8C79-72E54CB34424}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0681FA3-368F-4C8A-B01C-4EE1E8141F28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="265">
   <si>
     <t xml:space="preserve">code couleur: </t>
   </si>
@@ -836,9 +836,6 @@
     <t>l'association JLCPCB avait été oublié (ou perdue)</t>
   </si>
   <si>
-    <t>capa 10uF 25V JLCPCB C15850??</t>
-  </si>
-  <si>
     <t>LDO 5V, associer JLCPCB C16106</t>
   </si>
   <si>
@@ -876,6 +873,9 @@
   </si>
   <si>
     <t>OPB 2020</t>
+  </si>
+  <si>
+    <t>capa 10uF 10V JLCPCB C15850??</t>
   </si>
 </sst>
 </file>
@@ -1212,9 +1212,6 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="12" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1226,6 +1223,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="12" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1614,7 +1614,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D93" sqref="D93"/>
+      <selection pane="bottomLeft" activeCell="J87" sqref="J87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1741,28 +1741,28 @@
       <c r="AB3" s="23"/>
     </row>
     <row r="4" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="53" t="s">
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="53"/>
-      <c r="I4" s="54" t="s">
+      <c r="H4" s="52"/>
+      <c r="I4" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="54"/>
-      <c r="K4" s="55" t="s">
+      <c r="J4" s="53"/>
+      <c r="K4" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="55"/>
-      <c r="M4" s="55"/>
-      <c r="N4" s="55"/>
+      <c r="L4" s="54"/>
+      <c r="M4" s="54"/>
+      <c r="N4" s="54"/>
       <c r="O4" s="22" t="s">
         <v>11</v>
       </c>
@@ -5395,7 +5395,7 @@
       <c r="AB77" s="10"/>
     </row>
     <row r="78" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A78" s="14" t="s">
+      <c r="A78" s="12" t="s">
         <v>34</v>
       </c>
       <c r="B78" s="7" t="s">
@@ -5419,8 +5419,12 @@
       <c r="H78" s="8"/>
       <c r="I78" s="45"/>
       <c r="J78" s="8"/>
-      <c r="K78" s="7"/>
-      <c r="L78" s="8"/>
+      <c r="K78" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L78" s="8">
+        <v>43982</v>
+      </c>
       <c r="M78" s="9"/>
       <c r="N78" s="9"/>
       <c r="O78" s="9"/>
@@ -5492,7 +5496,7 @@
         <v>146</v>
       </c>
       <c r="C80" s="46" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D80" s="7" t="s">
         <v>102</v>
@@ -5538,7 +5542,7 @@
         <v>146</v>
       </c>
       <c r="C81" s="46" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D81" s="7" t="s">
         <v>102</v>
@@ -5584,7 +5588,7 @@
         <v>146</v>
       </c>
       <c r="C82" s="46" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D82" s="7" t="s">
         <v>102</v>
@@ -5630,7 +5634,7 @@
         <v>146</v>
       </c>
       <c r="C83" s="46" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D83" s="7" t="s">
         <v>102</v>
@@ -5676,7 +5680,7 @@
         <v>146</v>
       </c>
       <c r="C84" s="46" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D84" s="7" t="s">
         <v>102</v>
@@ -5722,7 +5726,7 @@
         <v>146</v>
       </c>
       <c r="C85" s="46" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D85" s="7" t="s">
         <v>102</v>
@@ -5762,13 +5766,13 @@
     </row>
     <row r="86" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A86" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B86" s="43" t="s">
         <v>146</v>
       </c>
       <c r="C86" s="46" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D86" s="7" t="s">
         <v>102</v>
@@ -5814,7 +5818,7 @@
         <v>239</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D87" s="7" t="s">
         <v>232</v>
@@ -5899,7 +5903,7 @@
       <c r="AB88" s="10"/>
     </row>
     <row r="89" spans="1:28" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="17" t="s">
+      <c r="A89" s="12" t="s">
         <v>243</v>
       </c>
       <c r="B89" s="7" t="s">
@@ -5917,8 +5921,12 @@
       <c r="F89" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="G89" s="7"/>
-      <c r="H89" s="8"/>
+      <c r="G89" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H89" s="8">
+        <v>43982</v>
+      </c>
       <c r="I89" s="7"/>
       <c r="J89" s="8"/>
       <c r="K89" s="7"/>
@@ -5983,14 +5991,14 @@
       <c r="AB90" s="10"/>
     </row>
     <row r="91" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A91" s="51">
+      <c r="A91" s="55">
         <v>885012107010</v>
       </c>
       <c r="B91" s="7" t="s">
         <v>146</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="D91" s="7" t="s">
         <v>76</v>
@@ -6001,8 +6009,12 @@
       <c r="F91" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="G91" s="7"/>
-      <c r="H91" s="8"/>
+      <c r="G91" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H91" s="8">
+        <v>43982</v>
+      </c>
       <c r="I91" s="7"/>
       <c r="J91" s="8"/>
       <c r="K91" s="7"/>
@@ -6032,7 +6044,7 @@
         <v>146</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D92" s="7" t="s">
         <v>102</v>
@@ -6070,13 +6082,13 @@
     </row>
     <row r="93" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A93" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B93" s="7" t="s">
         <v>140</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D93" s="7" t="s">
         <v>56</v>
@@ -6085,7 +6097,7 @@
         <v>56</v>
       </c>
       <c r="F93" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G93" s="7" t="s">
         <v>27</v>

</xml_diff>